<commit_message>
added test routines for mirenvelope and sig.envelope. Renamed test script files to corresponding names in mirtoolbox
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emon1\Documents\MATLAB\Workspace\RITMO\miningsuite\migrationTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CEA840-0572-4C55-8654-F307E363FFBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57904F6E-210F-4225-BB74-D9B43FF559B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17820" windowHeight="7845" xr2:uid="{385B2D26-0F6A-4802-9C4B-5EDD055393C7}"/>
+    <workbookView xWindow="450" yWindow="210" windowWidth="17550" windowHeight="11250" xr2:uid="{385B2D26-0F6A-4802-9C4B-5EDD055393C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
   <si>
     <t>mirtoolbox</t>
   </si>
@@ -259,6 +258,111 @@
   </si>
   <si>
     <t>FAIL for all h = 1, 2 3</t>
+  </si>
+  <si>
+    <t>mirenvelope</t>
+  </si>
+  <si>
+    <t>sig.envelope</t>
+  </si>
+  <si>
+    <t>…, 'Filter'</t>
+  </si>
+  <si>
+    <t>…, 'Hilbert'</t>
+  </si>
+  <si>
+    <t>..., 'Spectro'</t>
+  </si>
+  <si>
+    <t>…, 'FilterType', 'IIR'</t>
+  </si>
+  <si>
+    <t>…, 'FilterType', 'HalfHann'</t>
+  </si>
+  <si>
+    <t>…, 'FilterType', 'Butter'</t>
+  </si>
+  <si>
+    <t>…, 'CutOff', c</t>
+  </si>
+  <si>
+    <t>…, 'Tau', t</t>
+  </si>
+  <si>
+    <t>…, 'PostDecim', N</t>
+  </si>
+  <si>
+    <t>…, 'PreSilence'</t>
+  </si>
+  <si>
+    <t>…, 'PostSilence'</t>
+  </si>
+  <si>
+    <t>..., ‘Frame’, .1, ‘s’, .1, ‘/1’, ‘Window’, ‘hanning’, b</t>
+  </si>
+  <si>
+    <t>…,'Frame'</t>
+  </si>
+  <si>
+    <t>…, 'UpSample', N</t>
+  </si>
+  <si>
+    <t>…, 'Complex'</t>
+  </si>
+  <si>
+    <t>…, 'Terhardt'</t>
+  </si>
+  <si>
+    <t>…, ''PowerSpectrum'</t>
+  </si>
+  <si>
+    <t>…, TimeSmooth', n</t>
+  </si>
+  <si>
+    <t>..., 'Sampling', r</t>
+  </si>
+  <si>
+    <t>…, 'Halfwave'</t>
+  </si>
+  <si>
+    <t>…, 'HalfwaveCenter'</t>
+  </si>
+  <si>
+    <t>…, 'Log'</t>
+  </si>
+  <si>
+    <t>…, 'MinLog', ml</t>
+  </si>
+  <si>
+    <t>…, 'Mu', mu</t>
+  </si>
+  <si>
+    <t>…, 'Power'</t>
+  </si>
+  <si>
+    <t>…, 'Diff'</t>
+  </si>
+  <si>
+    <t>…, 'HalfwaveDiff'</t>
+  </si>
+  <si>
+    <t>…, 'Normal', 'AcrossSegments'</t>
+  </si>
+  <si>
+    <t>…, 'Lambda', l</t>
+  </si>
+  <si>
+    <t>…, 'Smooth', o</t>
+  </si>
+  <si>
+    <t>…, 'Gauss', o</t>
+  </si>
+  <si>
+    <t>…, 'Klapurio6'</t>
+  </si>
+  <si>
+    <t>…, 'PreDecim'</t>
   </si>
 </sst>
 </file>
@@ -302,9 +406,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,19 +724,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57388FE9-85EB-4D9B-86EC-FA14BBD9DF1C}">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="C58" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1079,6 +1184,394 @@
         <v>37</v>
       </c>
     </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="E49" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" t="s">
+        <v>85</v>
+      </c>
+      <c r="F51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>82</v>
+      </c>
+      <c r="E52" t="s">
+        <v>82</v>
+      </c>
+      <c r="F52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" t="s">
+        <v>83</v>
+      </c>
+      <c r="F53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" t="s">
+        <v>84</v>
+      </c>
+      <c r="F54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" t="s">
+        <v>80</v>
+      </c>
+      <c r="F56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>87</v>
+      </c>
+      <c r="F58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>88</v>
+      </c>
+      <c r="F59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" t="s">
+        <v>90</v>
+      </c>
+      <c r="F61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" t="s">
+        <v>91</v>
+      </c>
+      <c r="F62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>92</v>
+      </c>
+      <c r="E63" t="s">
+        <v>92</v>
+      </c>
+      <c r="F63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" t="s">
+        <v>95</v>
+      </c>
+      <c r="F66" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>96</v>
+      </c>
+      <c r="E67" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E68" t="s">
+        <v>97</v>
+      </c>
+      <c r="F68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>98</v>
+      </c>
+      <c r="E70" t="s">
+        <v>98</v>
+      </c>
+      <c r="F70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>99</v>
+      </c>
+      <c r="E71" t="s">
+        <v>99</v>
+      </c>
+      <c r="F71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>100</v>
+      </c>
+      <c r="E72" t="s">
+        <v>100</v>
+      </c>
+      <c r="F72" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" t="s">
+        <v>101</v>
+      </c>
+      <c r="F73" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>102</v>
+      </c>
+      <c r="E74" t="s">
+        <v>102</v>
+      </c>
+      <c r="F74" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" t="s">
+        <v>103</v>
+      </c>
+      <c r="F75" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" t="s">
+        <v>104</v>
+      </c>
+      <c r="F76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>105</v>
+      </c>
+      <c r="E78" t="s">
+        <v>105</v>
+      </c>
+      <c r="F78" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>106</v>
+      </c>
+      <c r="E79" t="s">
+        <v>106</v>
+      </c>
+      <c r="F79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+      <c r="E80" t="s">
+        <v>107</v>
+      </c>
+      <c r="F80" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>108</v>
+      </c>
+      <c r="E81" t="s">
+        <v>108</v>
+      </c>
+      <c r="F81" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>109</v>
+      </c>
+      <c r="F82" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modified all function comment/heading to conventional structure
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="174">
   <si>
     <t xml:space="preserve">mirtoolbox</t>
   </si>
@@ -67,15 +67,18 @@
     <t xml:space="preserve">…, 'Detrend', d</t>
   </si>
   <si>
+    <t xml:space="preserve">…, ‘FWR’</t>
+  </si>
+  <si>
     <t xml:space="preserve">…, 'FWR'</t>
   </si>
   <si>
+    <t xml:space="preserve">…, Frame, wu,hu</t>
+  </si>
+  <si>
     <t xml:space="preserve">…, Frame, w,wu, h, hu</t>
   </si>
   <si>
-    <t xml:space="preserve">…, 'Frame' , …</t>
-  </si>
-  <si>
     <t xml:space="preserve">…, 'Extract', t1,t2,u</t>
   </si>
   <si>
@@ -85,118 +88,118 @@
     <t xml:space="preserve">…, 'Extract', t1,t2,'sp'</t>
   </si>
   <si>
+    <t xml:space="preserve">…, 'Extract', t1,t2,u, f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Trim'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'TrimThreshold', t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'TrimThreshold' , t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'TrimStart'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'JustStart'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the parameter need 'Trim' required. Are they the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'TrimEnd'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'JustEnd'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'BothEnds'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Channel', c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need suitable example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FreqBand', b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Point', p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Dim', d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Label', lb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirframe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Length', w, 's'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FrameSize', w, 's'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Length', w, 'sp'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FrameSize', w, 'sp'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Hop', w, 's'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FrameHop', h, 's'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Hop', w, 'sp'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FrameHop', h, 'sp'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Hop', w, '%'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FrameHop', h, '%'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Hop', w, 'Hz'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FrameHop', h, 'Hz'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Hop', w, '/1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FrameHop', h, '/1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirfilterbank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.filterbank/aud.filterbank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Gammatone'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aud.filterbank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…</t>
+  </si>
+  <si>
     <t xml:space="preserve">FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Extract', t1,t2,u, f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Trim'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'TrimThreshold', t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'TrimThreshold' , t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'TrimStart'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'JustStart'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the parameter need 'Trim' required. Are they the same</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'TrimEnd'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'JustEnd'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'BothEnds'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Channel', c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">need suitable example</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FreqBand', b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Point', p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Dim', d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Label', lb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mirframe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig.frame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Length', w, 's'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FrameSize', w, 's'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Length', w, 'sp'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FrameSize', w, 'sp'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Hop', w, 's'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FrameHop', h, 's'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Hop', w, 'sp'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FrameHop', h, 'sp'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Hop', w, '%'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FrameHop', h, '%'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Hop', w, 'Hz'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FrameHop', h, 'Hz'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Hop', w, '/1'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FrameHop', h, '/1'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mirfilterbank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig.filterbank/aud.filterbank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Gammatone'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aud.filterbank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…</t>
   </si>
   <si>
     <t xml:space="preserve">…, 'Lowest', f</t>
@@ -652,10 +655,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G150"/>
+  <dimension ref="B2:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -745,35 +748,41 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="E10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>5</v>
@@ -781,13 +790,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,6 +855,9 @@
       <c r="E20" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="F20" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
@@ -862,21 +874,33 @@
       <c r="E22" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="F22" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="F23" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="F24" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="F25" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
@@ -893,16 +917,16 @@
       <c r="E27" s="0" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,6 +936,9 @@
       <c r="E29" s="0" t="s">
         <v>45</v>
       </c>
+      <c r="F29" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
@@ -964,31 +991,31 @@
         <v>58</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>57</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,7 +1023,7 @@
         <v>32</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>32</v>
@@ -1007,122 +1034,122 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="E40" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>57</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>57</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>57</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>57</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>5</v>
@@ -1130,10 +1157,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>5</v>
@@ -1141,10 +1168,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>5</v>
@@ -1152,10 +1179,10 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>5</v>
@@ -1163,10 +1190,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>5</v>
@@ -1174,10 +1201,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>5</v>
@@ -1185,10 +1212,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>5</v>
@@ -1196,10 +1223,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>5</v>
@@ -1207,10 +1234,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>5</v>
@@ -1218,13 +1245,13 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1264,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>13</v>
@@ -1245,7 +1272,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>13</v>
@@ -1253,32 +1280,32 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F63" s="0" t="s">
         <v>5</v>
@@ -1286,10 +1313,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F64" s="0" t="s">
         <v>5</v>
@@ -1297,10 +1324,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>5</v>
@@ -1308,7 +1335,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="0" t="s">
@@ -1317,10 +1344,10 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>5</v>
@@ -1328,10 +1355,10 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>5</v>
@@ -1339,10 +1366,10 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>5</v>
@@ -1361,10 +1388,10 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F71" s="0" t="s">
         <v>5</v>
@@ -1372,10 +1399,10 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>5</v>
@@ -1383,10 +1410,10 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F73" s="0" t="s">
         <v>5</v>
@@ -1394,7 +1421,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F74" s="0" t="s">
         <v>13</v>
@@ -1402,10 +1429,10 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>5</v>
@@ -1413,24 +1440,24 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1446,21 +1473,21 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>13</v>
@@ -1468,29 +1495,29 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>13</v>
@@ -1498,108 +1525,150 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F98" s="0" t="s">
         <v>13</v>
@@ -1607,39 +1676,51 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F103" s="0" t="s">
         <v>13</v>
@@ -1647,7 +1728,7 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F104" s="0" t="s">
         <v>13</v>
@@ -1655,291 +1736,349 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="F105" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="F108" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="F109" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="F110" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="F111" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="F112" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+      <c r="F113" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="F114" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="F115" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F133" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F141" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+      <c r="F143" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="F144" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="F145" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="F146" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
+      </c>
+      <c r="F147" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="F148" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="F149" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
+        <v>173</v>
+      </c>
+      <c r="F150" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added test routine for mirpeaks
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="203">
   <si>
     <t xml:space="preserve">mirtoolbox</t>
   </si>
@@ -542,6 +542,93 @@
   </si>
   <si>
     <t xml:space="preserve">…, ‘Median’,l, C, ‘Halfwave’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirsum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, ‘Center’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, ‘Mean’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirpeaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.peaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Total', m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Total', m, 'NoBegin'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Total', m, 'NoEnd'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Order', 'Amplitude'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Order', 'Abscissa'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Valleys'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Contrast', cthr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'SelectFirst', fthr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Contrast', cthr, 'SelectFirst', fthr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Threshold', thr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Valleys'. 'Threshold', thr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Interpol', 'no'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Interpol', 'Quadratic'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Reso', r </t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Reso', r, 'First'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, ‘Pref’, c, std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, ‘Nearest’, t, s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Normalize', 'Global' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Normalize', 'Local' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, ‘Extract’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…,’Only’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, ‘Track’, t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, ‘CollapseTracks’, t</t>
   </si>
 </sst>
 </file>
@@ -655,10 +742,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G1048576"/>
+  <dimension ref="B2:G179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A153" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F171" activeCellId="0" sqref="F171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2078,7 +2165,240 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D151" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C152" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E152" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C153" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E153" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C154" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="E154" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D155" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C156" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E156" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C157" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C158" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C159" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C160" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C161" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C162" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C163" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C164" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C165" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C166" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C167" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C168" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C169" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C170" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C171" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C172" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E172" s="2"/>
+      <c r="F172" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C173" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E173" s="2"/>
+      <c r="F173" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C174" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C175" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C176" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F176" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C177" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F177" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C178" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F178" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C179" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="F179" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
rechecked miraudio, mirenvelope and mirfilterbank
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="203">
   <si>
     <t xml:space="preserve">mirtoolbox</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">sig.signal</t>
   </si>
   <si>
+    <t xml:space="preserve">…</t>
+  </si>
+  <si>
     <t xml:space="preserve">OK</t>
   </si>
   <si>
@@ -64,9 +67,6 @@
     <t xml:space="preserve">NI</t>
   </si>
   <si>
-    <t xml:space="preserve">…, 'Detrend', d</t>
-  </si>
-  <si>
     <t xml:space="preserve">…, ‘FWR’</t>
   </si>
   <si>
@@ -79,9 +79,6 @@
     <t xml:space="preserve">…, Frame, w,wu, h, hu</t>
   </si>
   <si>
-    <t xml:space="preserve">…, 'Extract', t1,t2,u</t>
-  </si>
-  <si>
     <t xml:space="preserve">…, 'Extract', t1,t2,'s'</t>
   </si>
   <si>
@@ -94,45 +91,114 @@
     <t xml:space="preserve">…, 'Trim'</t>
   </si>
   <si>
-    <t xml:space="preserve">…, 'TrimThreshold', t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'TrimThreshold' , t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'TrimStart'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'JustStart'</t>
+    <t xml:space="preserve">…, ‘Trim’, 'TrimThreshold', t</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">‘Trim’,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'TrimThreshold' , t</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">…, ‘Trim’, 'TrimStart'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">‘Trim’,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'JustStart'</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Is the parameter need 'Trim' required. Are they the same</t>
   </si>
   <si>
-    <t xml:space="preserve">…, 'TrimEnd'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'JustEnd'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'BothEnds'</t>
+    <t xml:space="preserve">…, ‘Trim’, 'TrimEnd'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">‘Trim’,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'JustEnd'</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">…, 'Channel', c</t>
   </si>
   <si>
-    <t xml:space="preserve">need suitable example</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FreqBand', b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Point', p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Dim', d</t>
-  </si>
-  <si>
     <t xml:space="preserve">…, 'Label', lb</t>
   </si>
   <si>
@@ -196,46 +262,288 @@
     <t xml:space="preserve">aud.filterbank</t>
   </si>
   <si>
-    <t xml:space="preserve">…</t>
+    <t xml:space="preserve">…, ‘Gammatone’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Lowest', f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, '2Channels'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'NbChannels', N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Manual', f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.filterbank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'CutOff', f</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'Manual', f,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'Order', o</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'CutOff', f,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'Order', o</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'Manual', f,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'Hop', 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'CutOff', f,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'Hop', 1</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">FAIL</t>
   </si>
   <si>
-    <t xml:space="preserve">…, 'Lowest', f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, '2Channels'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'NbChannels', N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig.filterbank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Manual', f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'CutOff', f</t>
+    <t xml:space="preserve">FAIL for all h = 1, 2 3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'Manual', f,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'Hop', 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'CutOff', f,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'Hop', 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'Manual', f,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'Hop', 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">…, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'CutOff', f,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'Hop', 3</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Mel'</t>
   </si>
   <si>
     <t xml:space="preserve">ERROR</t>
   </si>
   <si>
-    <t xml:space="preserve">CutOff parameter not defined</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Order', o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Hop', h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAIL for all h = 1, 2 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Mel'</t>
+    <t xml:space="preserve">need implementation check</t>
   </si>
   <si>
     <t xml:space="preserve">…, 'Bark'</t>
@@ -274,7 +582,25 @@
     <t xml:space="preserve">…, 'FilterType', 'Butter'</t>
   </si>
   <si>
-    <t xml:space="preserve">…, 'CutOff', c</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">…, 'FilterType', 'Butter', </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'CutOff', c</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">…, 'PostDecim', N</t>
@@ -638,7 +964,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -668,6 +994,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -712,12 +1044,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -742,10 +1078,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G179"/>
+  <dimension ref="B2:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A153" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F171" activeCellId="0" sqref="F171"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -781,57 +1117,57 @@
       <c r="D4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="F6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="F9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,7 +1189,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,6 +1199,9 @@
       <c r="E12" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="F12" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
@@ -872,26 +1211,26 @@
         <v>20</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="E15" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="F15" s="0" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,1506 +1238,1519 @@
         <v>23</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E18" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>28</v>
+      <c r="F19" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="0" t="s">
+      <c r="B21" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="E22" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="E23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="E24" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>39</v>
+      <c r="C26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>5</v>
+      <c r="B29" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="E32" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="E33" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D36" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E36" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F35" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="0" t="s">
-        <v>60</v>
+      <c r="F36" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>57</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>62</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="D39" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D40" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="0" t="s">
-        <v>73</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>82</v>
+      <c r="C53" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>90</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>91</v>
+      <c r="C63" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>92</v>
-      </c>
+      <c r="C64" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" s="3"/>
       <c r="F64" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>93</v>
+      <c r="C65" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>95</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E66" s="2"/>
+      <c r="C66" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>96</v>
+      </c>
       <c r="F66" s="0" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>103</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="0" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E81" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>108</v>
+      <c r="B82" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>111</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>112</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>111</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>113</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="F87" s="0" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E96" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="E101" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E102" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>131</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F105" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E106" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F106" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="E107" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F107" s="0" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>140</v>
       </c>
       <c r="F112" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
+      </c>
+      <c r="E113" s="0" t="s">
+        <v>141</v>
       </c>
       <c r="F113" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E114" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="F114" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="F115" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="D116" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C116" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="E120" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E121" s="0" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D122" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="0" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
+      </c>
+      <c r="F131" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="F133" s="0" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
+      </c>
+      <c r="F139" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C140" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D140" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="0" t="s">
-        <v>166</v>
+        <v>144</v>
+      </c>
+      <c r="E141" s="0" t="s">
+        <v>144</v>
       </c>
       <c r="F141" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D142" s="0" t="s">
-        <v>168</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C142" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E142" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F142" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="0" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="F143" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="0" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="F144" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="E145" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F145" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E146" s="0" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="F146" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F147" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="F148" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C149" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="F149" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D149" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="F150" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="D151" s="0" t="s">
-        <v>175</v>
+        <v>5</v>
+      </c>
+      <c r="E150" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C151" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E151" s="0" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="0" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C153" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="E153" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D153" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="0" t="s">
-        <v>177</v>
+        <v>5</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B155" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="D155" s="0" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C156" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E156" s="0" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C155" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C156" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C157" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>180</v>
+      <c r="C157" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C158" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>181</v>
+      <c r="C158" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C159" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>182</v>
+      <c r="C159" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>183</v>
+      <c r="C160" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E161" s="2" t="s">
-        <v>184</v>
+      <c r="C161" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>185</v>
+      <c r="C162" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>186</v>
+      <c r="C163" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C164" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>187</v>
+      <c r="C164" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C165" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E165" s="2" t="s">
-        <v>188</v>
+      <c r="C165" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C166" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>189</v>
+      <c r="C166" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C167" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>190</v>
+      <c r="C167" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C168" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E168" s="2" t="s">
-        <v>191</v>
+      <c r="C168" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C169" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E169" s="2" t="s">
-        <v>192</v>
+      <c r="C169" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C170" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E170" s="2" t="s">
-        <v>193</v>
+      <c r="C170" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E170" s="3"/>
+      <c r="F170" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E171" s="2" t="s">
-        <v>194</v>
+      <c r="C171" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E171" s="3"/>
+      <c r="F171" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E172" s="2"/>
-      <c r="F172" s="0" t="s">
-        <v>13</v>
+      <c r="C172" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E173" s="2"/>
-      <c r="F173" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C174" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C175" s="2" t="s">
+      <c r="C173" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E175" s="2" t="s">
+      <c r="E173" s="3" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C174" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F174" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C175" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F175" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F176" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F177" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="F178" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C179" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="F179" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
fixed test for mirframe and test result successful
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="201">
   <si>
     <t xml:space="preserve">mirtoolbox</t>
   </si>
@@ -94,69 +94,13 @@
     <t xml:space="preserve">…, ‘Trim’, 'TrimThreshold', t</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">‘Trim’,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'TrimThreshold' , t</t>
-    </r>
+    <t xml:space="preserve">…, ‘Trim’,'TrimThreshold' , t</t>
   </si>
   <si>
     <t xml:space="preserve">…, ‘Trim’, 'TrimStart'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">‘Trim’,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'JustStart'</t>
-    </r>
+    <t xml:space="preserve">…, ‘Trim’,'JustStart'</t>
   </si>
   <si>
     <t xml:space="preserve">Is the parameter need 'Trim' required. Are they the same</t>
@@ -165,35 +109,7 @@
     <t xml:space="preserve">…, ‘Trim’, 'TrimEnd'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">‘Trim’,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'JustEnd'</t>
-    </r>
+    <t xml:space="preserve">…, ‘Trim’,'JustEnd'</t>
   </si>
   <si>
     <t xml:space="preserve">…, 'Channel', c</t>
@@ -235,9 +151,6 @@
     <t xml:space="preserve">…, 'Hop', w, '%'</t>
   </si>
   <si>
-    <t xml:space="preserve">…, 'FrameHop', h, '%'</t>
-  </si>
-  <si>
     <t xml:space="preserve">…, 'Hop', w, 'Hz'</t>
   </si>
   <si>
@@ -283,258 +196,31 @@
     <t xml:space="preserve">…, 'CutOff', f</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'Manual', f,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'Order', o</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'CutOff', f,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'Order', o</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'Manual', f,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'Hop', 1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'CutOff', f,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'Hop', 1</t>
-    </r>
+    <t xml:space="preserve">…, 'Manual', f,'Order', o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'CutOff', f,'Order', o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Manual', f,'Hop', 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'CutOff', f,'Hop', 1</t>
   </si>
   <si>
     <t xml:space="preserve">FAIL</t>
   </si>
   <si>
-    <t xml:space="preserve">FAIL for all h = 1, 2 3</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'Manual', f,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'Hop', 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'CutOff', f,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'Hop', 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'Manual', f,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'Hop', 3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">…, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'CutOff', f,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'Hop', 3</t>
-    </r>
+    <t xml:space="preserve">…, 'Manual', f,'Hop', 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'CutOff', f,'Hop', 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Manual', f,'Hop', 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'CutOff', f,'Hop', 3</t>
   </si>
   <si>
     <t xml:space="preserve">…, 'Mel'</t>
@@ -582,25 +268,7 @@
     <t xml:space="preserve">…, 'FilterType', 'Butter'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">…, 'FilterType', 'Butter', </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'CutOff', c</t>
-    </r>
+    <t xml:space="preserve">…, 'FilterType', 'Butter', 'CutOff', c</t>
   </si>
   <si>
     <t xml:space="preserve">…, 'PostDecim', N</t>
@@ -964,7 +632,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -994,12 +662,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1044,16 +706,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1080,8 +738,8 @@
   </sheetPr>
   <dimension ref="B2:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1317,6 +975,9 @@
       <c r="E23" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="F23" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
@@ -1336,48 +997,57 @@
       <c r="E25" s="0" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>43</v>
+      <c r="F26" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="0" t="s">
-        <v>45</v>
+      <c r="F27" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="0" t="s">
-        <v>47</v>
+      <c r="F28" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>6</v>
@@ -1385,13 +1055,13 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>6</v>
@@ -1399,13 +1069,13 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>6</v>
@@ -1413,13 +1083,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>6</v>
@@ -1430,7 +1100,7 @@
         <v>30</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>30</v>
@@ -1439,50 +1109,60 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="E36" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E38" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,13 +1170,13 @@
         <v>65</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>66</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,88 +1184,85 @@
         <v>67</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E40" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="0" t="s">
-        <v>63</v>
+      <c r="G40" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E42" s="0" t="s">
+      <c r="D43" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="0" t="s">
+      <c r="F43" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="0" t="s">
+      <c r="D44" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="C45" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="E45" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="0" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="E46" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>6</v>
@@ -1593,10 +1270,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>6</v>
@@ -1604,10 +1281,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>6</v>
@@ -1615,10 +1292,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>6</v>
@@ -1626,10 +1303,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>6</v>
@@ -1637,32 +1314,32 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E52" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F51" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="0" t="s">
+      <c r="F52" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E53" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>6</v>
@@ -1670,29 +1347,26 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>14</v>
@@ -1700,7 +1374,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>14</v>
@@ -1708,82 +1382,85 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="E62" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F61" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="0" t="s">
+      <c r="F62" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C63" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E62" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="3" t="s">
+      <c r="E63" s="2"/>
+      <c r="F63" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E64" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F63" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E64" s="3"/>
       <c r="F64" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>6</v>
@@ -1791,10 +1468,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F66" s="0" t="s">
         <v>6</v>
@@ -1802,10 +1479,10 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>6</v>
@@ -1813,10 +1490,10 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>6</v>
@@ -1824,10 +1501,10 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>6</v>
@@ -1835,147 +1512,147 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="E70" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="0" t="s">
+      <c r="F71" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="E71" s="0" t="s">
+      <c r="E72" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F71" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="F72" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="E80" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C81" s="0" t="s">
+      <c r="D81" s="0" t="s">
         <v>109</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="s">
+      <c r="C82" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="E82" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="F82" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="0" t="s">
-        <v>112</v>
-      </c>
       <c r="E83" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>6</v>
@@ -1983,34 +1660,45 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="E86" s="0" t="s">
+      <c r="E87" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F86" s="0" t="s">
+      <c r="F87" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2022,7 +1710,7 @@
         <v>116</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2044,7 +1732,7 @@
         <v>118</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,15 +1768,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E94" s="0" t="s">
-        <v>122</v>
-      </c>
       <c r="F94" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2102,12 +1787,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
         <v>124</v>
       </c>
+      <c r="E96" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="F96" s="0" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,45 +1817,45 @@
         <v>126</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="E99" s="0" t="s">
-        <v>127</v>
-      </c>
       <c r="F99" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="E100" s="0" t="s">
-        <v>128</v>
-      </c>
       <c r="F100" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="0" t="s">
         <v>129</v>
       </c>
+      <c r="E101" s="0" t="s">
+        <v>129</v>
+      </c>
       <c r="F101" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="E102" s="0" t="s">
+        <v>130</v>
+      </c>
       <c r="F102" s="0" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,29 +1866,23 @@
         <v>131</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="E104" s="0" t="s">
-        <v>132</v>
-      </c>
       <c r="F104" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E105" s="0" t="s">
-        <v>133</v>
-      </c>
       <c r="F105" s="0" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,49 +1917,49 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="0" t="s">
         <v>138</v>
       </c>
+      <c r="E110" s="0" t="s">
+        <v>138</v>
+      </c>
       <c r="F110" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="0" t="s">
         <v>139</v>
       </c>
+      <c r="E111" s="0" t="s">
+        <v>139</v>
+      </c>
       <c r="F111" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E112" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="F112" s="0" t="s">
-        <v>6</v>
+      <c r="D112" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="F113" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D114" s="0" t="s">
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C114" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E114" s="0" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2305,46 +1987,40 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="0" t="s">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="E118" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D118" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E119" s="0" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="0" t="s">
+      <c r="C120" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C121" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D120" s="0" t="s">
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="0" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="0" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="0" t="s">
         <v>152</v>
       </c>
@@ -2366,25 +2042,25 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="0" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
+      </c>
+      <c r="F129" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="F131" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,7 +2068,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="0" t="s">
         <v>160</v>
       </c>
@@ -2416,34 +2092,46 @@
       <c r="C137" s="0" t="s">
         <v>164</v>
       </c>
+      <c r="F137" s="0" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="0" t="s">
+      <c r="B138" s="0" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D138" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="0" t="s">
-        <v>166</v>
+        <v>142</v>
+      </c>
+      <c r="E139" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="F139" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C140" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="D140" s="0" t="s">
-        <v>168</v>
+      <c r="E140" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="F140" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="0" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="F141" s="0" t="s">
         <v>6</v>
@@ -2451,40 +2139,34 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E142" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F142" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C143" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="E142" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="F142" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C143" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="E143" s="0" t="s">
-        <v>170</v>
-      </c>
       <c r="F143" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E144" s="0" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="F144" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F145" s="0" t="s">
         <v>14</v>
@@ -2492,228 +2174,228 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="0" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="F146" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="0" t="s">
+      <c r="B147" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="F147" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D147" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="F148" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E148" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C149" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="D149" s="0" t="s">
-        <v>175</v>
+      <c r="E149" s="0" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E150" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D151" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C152" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E150" s="0" t="s">
+      <c r="E152" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="E151" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C152" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="E152" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="0" t="s">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C153" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D153" s="0" t="s">
+      <c r="E153" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C154" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C154" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="E154" s="0" t="s">
-        <v>5</v>
+      <c r="E154" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C155" s="3" t="s">
+      <c r="C155" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E155" s="3" t="s">
+      <c r="E155" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C156" s="3" t="s">
+      <c r="C156" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E156" s="3" t="s">
+      <c r="E156" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C157" s="3" t="s">
+      <c r="C157" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E157" s="3" t="s">
+      <c r="E157" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C158" s="3" t="s">
+      <c r="C158" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E158" s="3" t="s">
+      <c r="E158" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C159" s="3" t="s">
+      <c r="C159" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E159" s="3" t="s">
+      <c r="E159" s="2" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="3" t="s">
+      <c r="C160" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E160" s="3" t="s">
+      <c r="E160" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="3" t="s">
+      <c r="C161" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E161" s="3" t="s">
+      <c r="E161" s="2" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="3" t="s">
+      <c r="C162" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E162" s="3" t="s">
+      <c r="E162" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="3" t="s">
+      <c r="C163" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="E163" s="2" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C164" s="3" t="s">
+      <c r="C164" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E164" s="3" t="s">
+      <c r="E164" s="2" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C165" s="3" t="s">
+      <c r="C165" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E165" s="3" t="s">
+      <c r="E165" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C166" s="3" t="s">
+      <c r="C166" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E166" s="3" t="s">
+      <c r="E166" s="2" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C167" s="3" t="s">
+      <c r="C167" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E167" s="3" t="s">
+      <c r="E167" s="2" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C168" s="3" t="s">
+      <c r="C168" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E168" s="3" t="s">
-        <v>193</v>
+      <c r="E168" s="2"/>
+      <c r="F168" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C169" s="3" t="s">
+      <c r="C169" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E169" s="3" t="s">
-        <v>194</v>
+      <c r="E169" s="2"/>
+      <c r="F169" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C170" s="3" t="s">
+      <c r="C170" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E170" s="3"/>
-      <c r="F170" s="0" t="s">
-        <v>14</v>
+      <c r="E170" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="3" t="s">
+      <c r="C171" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E171" s="3"/>
-      <c r="F171" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="3" t="s">
+      <c r="E171" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C172" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="E172" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="3" t="s">
+      <c r="F172" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C173" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="E173" s="3" t="s">
-        <v>198</v>
+      <c r="F173" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2732,22 +2414,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C176" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="F176" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C177" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="F177" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
updated test on mirsum
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="204">
   <si>
     <t xml:space="preserve">mirtoolbox</t>
   </si>
@@ -103,9 +103,6 @@
     <t xml:space="preserve">…, ‘Trim’,'JustStart'</t>
   </si>
   <si>
-    <t xml:space="preserve">Is the parameter need 'Trim' required. Are they the same</t>
-  </si>
-  <si>
     <t xml:space="preserve">…, ‘Trim’, 'TrimEnd'</t>
   </si>
   <si>
@@ -544,10 +541,22 @@
     <t xml:space="preserve">sig.sum</t>
   </si>
   <si>
-    <t xml:space="preserve">…, ‘Center’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, ‘Mean’</t>
+    <t xml:space="preserve">mirenvelope(mirfilterbank(...))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.envelope(sig.filterbank(...))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirenvelope(mirfilterbank(...)), 'Mean'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.envelope(sig.filterbank(...)), 'Mean'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirenvelope(mirautocor(...)), 'Mean'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.envelope(sig.autocor(...)), 'Mean'</t>
   </si>
   <si>
     <t xml:space="preserve">mirpeaks</t>
@@ -738,8 +747,8 @@
   </sheetPr>
   <dimension ref="B2:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C133" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F151" activeCellId="0" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -902,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
         <v>25</v>
       </c>
@@ -912,30 +921,24 @@
       <c r="F17" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="F18" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>6</v>
@@ -943,7 +946,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>14</v>
@@ -951,18 +954,18 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>6</v>
@@ -970,10 +973,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>6</v>
@@ -981,10 +984,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>6</v>
@@ -992,10 +995,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>6</v>
@@ -1003,7 +1006,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>14</v>
@@ -1011,10 +1014,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>6</v>
@@ -1022,10 +1025,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>6</v>
@@ -1033,63 +1036,60 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="0" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="E31" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="F31" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="0" t="s">
+      <c r="D32" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="D33" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>6</v>
@@ -1097,13 +1097,13 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>6</v>
@@ -1111,158 +1111,161 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="E36" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="F36" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="0" t="s">
+      <c r="D37" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="F37" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="0" t="s">
+      <c r="D38" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="F38" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>6</v>
+        <v>67</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="0" t="s">
+      <c r="D44" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="0" t="s">
+      <c r="F44" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+      <c r="D45" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="0" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="0" t="s">
-        <v>76</v>
-      </c>
       <c r="E46" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>6</v>
@@ -1270,10 +1273,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>6</v>
@@ -1281,10 +1284,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>6</v>
@@ -1292,10 +1295,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>6</v>
@@ -1303,10 +1306,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>6</v>
@@ -1314,32 +1317,32 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E53" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>83</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>6</v>
@@ -1347,26 +1350,29 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>22</v>
+        <v>83</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>14</v>
@@ -1374,7 +1380,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>14</v>
@@ -1382,54 +1388,51 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>91</v>
+      <c r="C62" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="F62" s="0" t="s">
         <v>6</v>
@@ -1437,30 +1440,30 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E63" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="F63" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>93</v>
-      </c>
+      <c r="C64" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" s="2"/>
       <c r="F64" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>6</v>
@@ -1468,10 +1471,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F66" s="0" t="s">
         <v>6</v>
@@ -1479,10 +1482,10 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>6</v>
@@ -1490,10 +1493,10 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>6</v>
@@ -1501,10 +1504,10 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>6</v>
@@ -1512,147 +1515,147 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E70" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>100</v>
-      </c>
       <c r="F72" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="F80" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0" t="s">
+      <c r="D82" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="F82" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="F81" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="E83" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>6</v>
@@ -1660,32 +1663,32 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F86" s="0" t="s">
         <v>6</v>
@@ -1693,10 +1696,10 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F87" s="0" t="s">
         <v>6</v>
@@ -1704,32 +1707,32 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F90" s="0" t="s">
         <v>6</v>
@@ -1737,10 +1740,10 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F91" s="0" t="s">
         <v>6</v>
@@ -1748,10 +1751,10 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F92" s="0" t="s">
         <v>6</v>
@@ -1759,127 +1762,130 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="E93" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="F93" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F94" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="E95" s="0" t="s">
-        <v>123</v>
-      </c>
       <c r="F95" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F98" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>125</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F100" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E101" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>130</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F105" s="0" t="s">
         <v>14</v>
@@ -1887,7 +1893,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="0" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F106" s="0" t="s">
         <v>14</v>
@@ -1895,7 +1901,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="0" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F107" s="0" t="s">
         <v>14</v>
@@ -1903,7 +1909,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="0" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F108" s="0" t="s">
         <v>14</v>
@@ -1911,216 +1917,213 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F109" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E110" s="0" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F111" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F112" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="E111" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="F111" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="0" t="s">
+      <c r="D113" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="D112" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C113" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E113" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C118" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="E117" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="0" t="s">
+      <c r="D119" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="D118" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="0" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="0" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="0" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="0" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="0" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="0" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="F129" s="0" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F130" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="0" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C131" s="0" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="0" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="0" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="0" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="0" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="F138" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="F137" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="0" t="s">
+      <c r="D139" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="D138" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E139" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F139" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="0" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="F140" s="0" t="s">
         <v>6</v>
@@ -2128,10 +2131,10 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F141" s="0" t="s">
         <v>6</v>
@@ -2139,26 +2142,29 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="0" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="F142" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="0" t="s">
-        <v>169</v>
+        <v>145</v>
+      </c>
+      <c r="E143" s="0" t="s">
+        <v>145</v>
       </c>
       <c r="F143" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F144" s="0" t="s">
         <v>14</v>
@@ -2166,7 +2172,7 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="0" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F145" s="0" t="s">
         <v>14</v>
@@ -2174,192 +2180,200 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F146" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C147" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F147" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="F146" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="0" t="s">
+      <c r="D148" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="D147" s="0" t="s">
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C149" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C148" s="0" t="s">
+      <c r="E149" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F149" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C150" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F150" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C151" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F151" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D152" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C153" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E148" s="0" t="s">
+      <c r="E153" s="0" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C149" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="E149" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C150" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="E150" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="D151" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C152" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="E152" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C153" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C160" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C164" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C165" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E168" s="2"/>
-      <c r="F168" s="0" t="s">
-        <v>14</v>
+        <v>195</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E169" s="2"/>
       <c r="F169" s="0" t="s">
@@ -2368,31 +2382,32 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E170" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
+      </c>
+      <c r="E170" s="2"/>
+      <c r="F170" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F172" s="0" t="s">
-        <v>14</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C172" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C173" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F173" s="0" t="s">
         <v>14</v>
@@ -2400,7 +2415,7 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F174" s="0" t="s">
         <v>14</v>
@@ -2408,13 +2423,20 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C175" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F175" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C176" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="F176" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
attempted to extract data for mirpeaks. Need to check if implementation is correct. Test fail now shows in red
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -148,6 +148,9 @@
     <t xml:space="preserve">…, 'Hop', w, '%'</t>
   </si>
   <si>
+    <t xml:space="preserve">…, 'FrameHop', h, '%'</t>
+  </si>
+  <si>
     <t xml:space="preserve">…, 'Hop', w, 'Hz'</t>
   </si>
   <si>
@@ -205,85 +208,82 @@
     <t xml:space="preserve">…, 'CutOff', f,'Hop', 1</t>
   </si>
   <si>
+    <t xml:space="preserve">…, 'Manual', f,'Hop', 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'CutOff', f,'Hop', 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Manual', f,'Hop', 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'CutOff', f,'Hop', 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Mel'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Bark'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Scheirer'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Klapuri'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirenvelope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig.envelope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Filter'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Hilbert'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'PreDecim'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FilterType', 'IIR'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'Tau', t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FilterType', 'HalfHann'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FilterType', 'Butter'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'FilterType', 'Butter', 'CutOff', c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'PostDecim', N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., 'Spectro'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'PreSilence'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…, 'PostSilence'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">..., ‘Frame’, .1, ‘s’, .1, ‘/1’, ‘Window’, ‘hanning’, b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…,'Frame'</t>
+  </si>
+  <si>
     <t xml:space="preserve">FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Manual', f,'Hop', 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'CutOff', f,'Hop', 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Manual', f,'Hop', 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'CutOff', f,'Hop', 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Mel'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">need implementation check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Bark'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Scheirer'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Klapuri'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mirenvelope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig.envelope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Filter'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Hilbert'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'PreDecim'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FilterType', 'IIR'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'Tau', t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FilterType', 'HalfHann'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FilterType', 'Butter'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'FilterType', 'Butter', 'CutOff', c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'PostDecim', N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">..., 'Spectro'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'PreSilence'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…, 'PostSilence'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">..., ‘Frame’, .1, ‘s’, .1, ‘/1’, ‘Window’, ‘hanning’, b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…,'Frame'</t>
   </si>
   <si>
     <t xml:space="preserve">…, 'UpSample', N</t>
@@ -745,10 +745,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G1048576"/>
+  <dimension ref="B2:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C133" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F151" activeCellId="0" sqref="F151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1008,16 +1008,19 @@
       <c r="C26" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="E26" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="F26" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>6</v>
@@ -1025,10 +1028,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>6</v>
@@ -1036,10 +1039,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,13 +1058,13 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>6</v>
@@ -1069,13 +1072,13 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>6</v>
@@ -1083,13 +1086,13 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>6</v>
@@ -1097,13 +1100,13 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>6</v>
@@ -1114,7 +1117,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>29</v>
@@ -1125,13 +1128,13 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>6</v>
@@ -1139,13 +1142,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>6</v>
@@ -1153,16 +1156,16 @@
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,13 +1173,13 @@
         <v>62</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>63</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1184,41 +1187,38 @@
         <v>64</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>65</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>66</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>6</v>
@@ -1226,13 +1226,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>6</v>
@@ -1240,13 +1240,13 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>6</v>
@@ -1254,18 +1254,18 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>6</v>
@@ -1273,10 +1273,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>6</v>
@@ -1284,10 +1284,10 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>6</v>
@@ -1295,10 +1295,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>6</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>6</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>6</v>
@@ -1328,10 +1328,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>6</v>
@@ -1339,10 +1339,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>6</v>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>6</v>
@@ -1361,13 +1361,13 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,7 +1380,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>14</v>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>14</v>
@@ -1396,24 +1396,24 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F60" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,7 +1562,7 @@
         <v>100</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,7 +1573,7 @@
         <v>101</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,7 +1595,7 @@
         <v>102</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,7 +1617,7 @@
         <v>104</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,7 +1628,7 @@
         <v>105</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,7 +1680,7 @@
         <v>111</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,7 +1724,7 @@
         <v>115</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,7 +1809,7 @@
         <v>123</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,7 +1858,7 @@
         <v>128</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,7 +1869,7 @@
         <v>129</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,7 +1880,7 @@
         <v>130</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,7 +2064,7 @@
         <v>155</v>
       </c>
       <c r="F130" s="0" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,7 +2107,7 @@
         <v>163</v>
       </c>
       <c r="F138" s="0" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2232,7 @@
         <v>178</v>
       </c>
       <c r="F151" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated migration.xlsb with comment for each error
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emon1\Documents\MATLAB\toolbox\miningsuite\migrationTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C98CEA9-8B92-43AD-B82C-0594A40D3ABA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A13242C-9B57-4980-A9B7-59E10EBDC187}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="990" windowWidth="19460" windowHeight="9040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="240">
   <si>
     <t>mirtoolbox</t>
   </si>
@@ -693,9 +693,6 @@
     <t>maximum absolute difference : 12327.9033</t>
   </si>
   <si>
-    <t>dimension error</t>
-  </si>
-  <si>
     <t>maximum absolute difference : 4.0075e-12</t>
   </si>
   <si>
@@ -720,22 +717,34 @@
     <t>Needs implementation check</t>
   </si>
   <si>
-    <t>dimension error (596x1, 595x1)</t>
-  </si>
-  <si>
     <t>maximum absolute difference: 0.00037173</t>
   </si>
   <si>
-    <t>dimension error(131073x1, 131074x1)</t>
-  </si>
-  <si>
-    <t>significant dimension error (131073x1, 130800x1); values significantly different</t>
-  </si>
-  <si>
     <t>value in miningsuite = 10 x value in mirtoolbox</t>
   </si>
   <si>
     <t>significant data error</t>
+  </si>
+  <si>
+    <t>dimension error (596, 595)</t>
+  </si>
+  <si>
+    <t>significant dimension error (131073, 130800); values significantly different</t>
+  </si>
+  <si>
+    <t>dimension error(131073, 131074)</t>
+  </si>
+  <si>
+    <t>dimension error(11517, 11518)</t>
+  </si>
+  <si>
+    <t>significant dimension error (11517, 11532)</t>
+  </si>
+  <si>
+    <t>implementation error</t>
+  </si>
+  <si>
+    <t>dimension error (miningsuite with 0x0)</t>
   </si>
 </sst>
 </file>
@@ -1140,19 +1149,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G111" sqref="G111"/>
+    <sheetView tabSelected="1" topLeftCell="B76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.1796875" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="44.7265625" customWidth="1"/>
-    <col min="4" max="4" width="26.7265625" customWidth="1"/>
-    <col min="5" max="5" width="44.7265625" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" customWidth="1"/>
-    <col min="7" max="7" width="52.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.36328125" customWidth="1"/>
     <col min="8" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1200,7 +1209,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
@@ -1211,7 +1220,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
@@ -1222,7 +1231,7 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
@@ -1233,7 +1242,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
@@ -1252,7 +1261,7 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
@@ -1263,7 +1272,7 @@
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
@@ -1274,7 +1283,7 @@
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.35">
@@ -1285,7 +1294,7 @@
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.35">
@@ -1304,7 +1313,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
@@ -1315,7 +1324,7 @@
         <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
@@ -1326,7 +1335,7 @@
         <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
@@ -1337,7 +1346,7 @@
         <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
@@ -1348,7 +1357,7 @@
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
@@ -1383,7 +1392,7 @@
         <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
@@ -1394,7 +1403,7 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
@@ -1405,7 +1414,7 @@
         <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.35">
@@ -1416,7 +1425,7 @@
         <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
@@ -1427,7 +1436,7 @@
         <v>40</v>
       </c>
       <c r="F26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
@@ -1438,7 +1447,7 @@
         <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
@@ -1449,7 +1458,7 @@
         <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
@@ -1472,7 +1481,7 @@
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
@@ -1486,7 +1495,7 @@
         <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
@@ -1500,7 +1509,7 @@
         <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
@@ -1514,7 +1523,7 @@
         <v>51</v>
       </c>
       <c r="F33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.35">
@@ -1528,7 +1537,7 @@
         <v>52</v>
       </c>
       <c r="F34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.35">
@@ -1542,7 +1551,7 @@
         <v>27</v>
       </c>
       <c r="F35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.35">
@@ -1556,7 +1565,7 @@
         <v>55</v>
       </c>
       <c r="F36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
@@ -1570,7 +1579,7 @@
         <v>57</v>
       </c>
       <c r="F37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.35">
@@ -1584,7 +1593,7 @@
         <v>59</v>
       </c>
       <c r="F38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
@@ -1598,7 +1607,7 @@
         <v>61</v>
       </c>
       <c r="F39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.35">
@@ -1612,7 +1621,7 @@
         <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.35">
@@ -1626,7 +1635,7 @@
         <v>64</v>
       </c>
       <c r="F41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.35">
@@ -1640,7 +1649,7 @@
         <v>65</v>
       </c>
       <c r="F42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.35">
@@ -1654,7 +1663,7 @@
         <v>66</v>
       </c>
       <c r="F43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.35">
@@ -1668,7 +1677,7 @@
         <v>67</v>
       </c>
       <c r="F44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.35">
@@ -1691,7 +1700,7 @@
         <v>70</v>
       </c>
       <c r="F46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
@@ -1702,7 +1711,7 @@
         <v>71</v>
       </c>
       <c r="F47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.35">
@@ -1713,7 +1722,7 @@
         <v>72</v>
       </c>
       <c r="F48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.35">
@@ -1724,7 +1733,7 @@
         <v>73</v>
       </c>
       <c r="F49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.35">
@@ -1735,7 +1744,7 @@
         <v>74</v>
       </c>
       <c r="F50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.35">
@@ -1746,7 +1755,7 @@
         <v>75</v>
       </c>
       <c r="F51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.35">
@@ -1757,7 +1766,7 @@
         <v>76</v>
       </c>
       <c r="F52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.35">
@@ -1768,7 +1777,7 @@
         <v>77</v>
       </c>
       <c r="F53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.35">
@@ -1779,7 +1788,7 @@
         <v>78</v>
       </c>
       <c r="F54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.35">
@@ -1790,7 +1799,7 @@
         <v>79</v>
       </c>
       <c r="F55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.35">
@@ -1836,7 +1845,7 @@
         <v>209</v>
       </c>
       <c r="F60" t="s">
-        <v>83</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.35">
@@ -1847,7 +1856,7 @@
         <v>84</v>
       </c>
       <c r="F61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.35">
@@ -1858,7 +1867,7 @@
         <v>85</v>
       </c>
       <c r="F62" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.35">
@@ -1869,7 +1878,7 @@
         <v>86</v>
       </c>
       <c r="F63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.35">
@@ -1881,7 +1890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" t="s">
         <v>88</v>
       </c>
@@ -1889,10 +1898,10 @@
         <v>88</v>
       </c>
       <c r="F65" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" t="s">
         <v>89</v>
       </c>
@@ -1900,10 +1909,10 @@
         <v>89</v>
       </c>
       <c r="F66" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" t="s">
         <v>90</v>
       </c>
@@ -1911,10 +1920,10 @@
         <v>90</v>
       </c>
       <c r="F67" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" t="s">
         <v>8</v>
       </c>
@@ -1922,10 +1931,10 @@
         <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" t="s">
         <v>91</v>
       </c>
@@ -1933,10 +1942,10 @@
         <v>91</v>
       </c>
       <c r="F69" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" t="s">
         <v>92</v>
       </c>
@@ -1944,10 +1953,10 @@
         <v>92</v>
       </c>
       <c r="F70" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" t="s">
         <v>93</v>
       </c>
@@ -1955,10 +1964,10 @@
         <v>93</v>
       </c>
       <c r="F71" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" t="s">
         <v>94</v>
       </c>
@@ -1969,10 +1978,10 @@
         <v>94</v>
       </c>
       <c r="F72" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" t="s">
         <v>95</v>
       </c>
@@ -1980,10 +1989,10 @@
         <v>95</v>
       </c>
       <c r="F73" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" t="s">
         <v>96</v>
       </c>
@@ -1993,8 +2002,11 @@
       <c r="F74" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="G74" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" t="s">
         <v>97</v>
       </c>
@@ -2004,8 +2016,11 @@
       <c r="F75" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="G75" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" t="s">
         <v>11</v>
       </c>
@@ -2013,10 +2028,10 @@
         <v>11</v>
       </c>
       <c r="F76" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" t="s">
         <v>98</v>
       </c>
@@ -2026,8 +2041,11 @@
       <c r="F77" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="G77" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" t="s">
         <v>99</v>
       </c>
@@ -2038,10 +2056,10 @@
         <v>99</v>
       </c>
       <c r="F78" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" t="s">
         <v>100</v>
       </c>
@@ -2051,8 +2069,11 @@
       <c r="F79" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="G79" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" t="s">
         <v>101</v>
       </c>
@@ -2061,6 +2082,9 @@
       </c>
       <c r="F80" t="s">
         <v>83</v>
+      </c>
+      <c r="G80" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.35">
@@ -2081,7 +2105,7 @@
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G82" s="5"/>
     </row>
@@ -2093,7 +2117,7 @@
         <v>105</v>
       </c>
       <c r="F83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.35">
@@ -2104,7 +2128,7 @@
         <v>106</v>
       </c>
       <c r="F84" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.35">
@@ -2118,7 +2142,7 @@
         <v>83</v>
       </c>
       <c r="G85" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.35">
@@ -2129,7 +2153,7 @@
         <v>108</v>
       </c>
       <c r="F86" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.35">
@@ -2140,7 +2164,7 @@
         <v>109</v>
       </c>
       <c r="F87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.35">
@@ -2151,7 +2175,7 @@
         <v>110</v>
       </c>
       <c r="F88" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.35">
@@ -2176,7 +2200,7 @@
         <v>112</v>
       </c>
       <c r="F90" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.35">
@@ -2187,7 +2211,7 @@
         <v>113</v>
       </c>
       <c r="F91" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.35">
@@ -2198,7 +2222,7 @@
         <v>114</v>
       </c>
       <c r="F92" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.35">
@@ -2209,7 +2233,7 @@
         <v>115</v>
       </c>
       <c r="F93" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.35">
@@ -2220,7 +2244,7 @@
         <v>116</v>
       </c>
       <c r="F94" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.35">
@@ -2239,7 +2263,7 @@
         <v>118</v>
       </c>
       <c r="F96" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.35">
@@ -2253,7 +2277,7 @@
         <v>83</v>
       </c>
       <c r="G97" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.35">
@@ -2264,7 +2288,7 @@
         <v>120</v>
       </c>
       <c r="F98" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.35">
@@ -2275,7 +2299,7 @@
         <v>121</v>
       </c>
       <c r="F99" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.35">
@@ -2305,7 +2329,7 @@
         <v>83</v>
       </c>
       <c r="G102" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.35">
@@ -2319,7 +2343,7 @@
         <v>83</v>
       </c>
       <c r="G103" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.35">
@@ -2333,7 +2357,7 @@
         <v>83</v>
       </c>
       <c r="G104" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.35">
@@ -2392,7 +2416,7 @@
         <v>133</v>
       </c>
       <c r="F111" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.35">
@@ -2403,7 +2427,7 @@
         <v>134</v>
       </c>
       <c r="F112" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.35">
@@ -2448,7 +2472,7 @@
         <v>139</v>
       </c>
       <c r="G116" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.35">
@@ -2459,7 +2483,7 @@
         <v>140</v>
       </c>
       <c r="G117" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.35">
@@ -2470,7 +2494,7 @@
         <v>141</v>
       </c>
       <c r="F118" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.35">
@@ -2594,6 +2618,9 @@
       <c r="F129" t="s">
         <v>83</v>
       </c>
+      <c r="G129" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C130" t="s">
@@ -2627,7 +2654,7 @@
         <v>154</v>
       </c>
       <c r="F133" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.35">
@@ -2693,7 +2720,7 @@
         <v>137</v>
       </c>
       <c r="F140" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.35">
@@ -2704,7 +2731,7 @@
         <v>162</v>
       </c>
       <c r="F141" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.35">
@@ -2715,7 +2742,7 @@
         <v>163</v>
       </c>
       <c r="F142" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.35">
@@ -2726,7 +2753,7 @@
         <v>141</v>
       </c>
       <c r="F143" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.35">
@@ -2781,7 +2808,7 @@
         <v>170</v>
       </c>
       <c r="F149" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.35">
@@ -2792,7 +2819,7 @@
         <v>172</v>
       </c>
       <c r="F150" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.35">
@@ -2826,7 +2853,7 @@
         <v>4</v>
       </c>
       <c r="F153" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.35">
@@ -2837,7 +2864,7 @@
         <v>177</v>
       </c>
       <c r="F154" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.35">
@@ -2848,7 +2875,7 @@
         <v>178</v>
       </c>
       <c r="F155" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="156" spans="2:7" x14ac:dyDescent="0.35">
@@ -2859,7 +2886,7 @@
         <v>179</v>
       </c>
       <c r="F156" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.35">
@@ -2870,7 +2897,7 @@
         <v>180</v>
       </c>
       <c r="F157" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.35">
@@ -2881,7 +2908,7 @@
         <v>181</v>
       </c>
       <c r="F158" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.35">
@@ -2892,7 +2919,7 @@
         <v>182</v>
       </c>
       <c r="F159" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="160" spans="2:7" x14ac:dyDescent="0.35">
@@ -2903,7 +2930,7 @@
         <v>183</v>
       </c>
       <c r="F160" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="161" spans="3:6" x14ac:dyDescent="0.35">
@@ -2914,7 +2941,7 @@
         <v>184</v>
       </c>
       <c r="F161" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="162" spans="3:6" x14ac:dyDescent="0.35">
@@ -2925,7 +2952,7 @@
         <v>185</v>
       </c>
       <c r="F162" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="163" spans="3:6" x14ac:dyDescent="0.35">
@@ -2936,7 +2963,7 @@
         <v>186</v>
       </c>
       <c r="F163" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="164" spans="3:6" x14ac:dyDescent="0.35">
@@ -2947,7 +2974,7 @@
         <v>187</v>
       </c>
       <c r="F164" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="165" spans="3:6" x14ac:dyDescent="0.35">
@@ -2958,7 +2985,7 @@
         <v>188</v>
       </c>
       <c r="F165" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="166" spans="3:6" x14ac:dyDescent="0.35">
@@ -2969,7 +2996,7 @@
         <v>189</v>
       </c>
       <c r="F166" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="167" spans="3:6" x14ac:dyDescent="0.35">
@@ -2980,7 +3007,7 @@
         <v>190</v>
       </c>
       <c r="F167" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="168" spans="3:6" x14ac:dyDescent="0.35">
@@ -2991,7 +3018,7 @@
         <v>191</v>
       </c>
       <c r="F168" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="169" spans="3:6" x14ac:dyDescent="0.35">
@@ -3020,7 +3047,7 @@
         <v>194</v>
       </c>
       <c r="F171" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="172" spans="3:6" x14ac:dyDescent="0.35">
@@ -3031,7 +3058,7 @@
         <v>195</v>
       </c>
       <c r="F172" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="173" spans="3:6" x14ac:dyDescent="0.35">
@@ -3084,65 +3111,68 @@
         <v>4</v>
       </c>
       <c r="F178" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C179" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E179" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F179" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C180" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E180" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F180" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G180" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C181" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E181" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F181" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C182" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E182" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F182" t="s">
         <v>83</v>
       </c>
+      <c r="G182" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="183" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C183" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E183" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F183" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="184" spans="2:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
moved basic operater files to a separate folder
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emon1\Documents\MATLAB\toolbox\miningsuite\migrationTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A13242C-9B57-4980-A9B7-59E10EBDC187}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87DF425-D21C-4B2F-9971-5C547B048CCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1070" yWindow="590" windowWidth="19200" windowHeight="8510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="241">
   <si>
     <t>mirtoolbox</t>
   </si>
@@ -745,6 +745,9 @@
   </si>
   <si>
     <t>dimension error (miningsuite with 0x0)</t>
+  </si>
+  <si>
+    <t>…, ‘Max’, max</t>
   </si>
 </sst>
 </file>
@@ -1149,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView tabSelected="1" topLeftCell="B159" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E170" sqref="E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2477,7 +2480,7 @@
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
-        <v>140</v>
+        <v>240</v>
       </c>
       <c r="E117" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
removed status of mirsegment tests since previous SUCCESS was due to mistakes. mirsegment needs further investigation
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emon1\Documents\MATLAB\toolbox\miningsuite\migrationTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87DF425-D21C-4B2F-9971-5C547B048CCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57544F70-04D9-46A0-A026-4CEED90D2FFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1070" yWindow="590" windowWidth="19200" windowHeight="8510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="19200" windowHeight="8510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="242">
   <si>
     <t>mirtoolbox</t>
   </si>
@@ -714,9 +714,6 @@
     <t>…, 'RMS'</t>
   </si>
   <si>
-    <t>Needs implementation check</t>
-  </si>
-  <si>
     <t>maximum absolute difference: 0.00037173</t>
   </si>
   <si>
@@ -748,13 +745,19 @@
   </si>
   <si>
     <t>…, ‘Max’, max</t>
+  </si>
+  <si>
+    <t>Basic Operators</t>
+  </si>
+  <si>
+    <t>Feature Extractors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -777,8 +780,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -788,6 +797,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -836,6 +851,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1150,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G190"/>
+  <dimension ref="B1:G192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B159" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E170" sqref="E170"/>
+    <sheetView tabSelected="1" topLeftCell="B130" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1168,29 +1186,39 @@
     <col min="8" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>201</v>
-      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="B3" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
@@ -2006,7 +2034,7 @@
         <v>83</v>
       </c>
       <c r="G74" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.35">
@@ -2020,7 +2048,7 @@
         <v>83</v>
       </c>
       <c r="G75" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.35">
@@ -2045,7 +2073,7 @@
         <v>83</v>
       </c>
       <c r="G77" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.35">
@@ -2073,7 +2101,7 @@
         <v>83</v>
       </c>
       <c r="G79" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.35">
@@ -2087,7 +2115,7 @@
         <v>83</v>
       </c>
       <c r="G80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.35">
@@ -2145,7 +2173,7 @@
         <v>83</v>
       </c>
       <c r="G85" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.35">
@@ -2192,7 +2220,7 @@
         <v>83</v>
       </c>
       <c r="G89" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.35">
@@ -2280,7 +2308,7 @@
         <v>83</v>
       </c>
       <c r="G97" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.35">
@@ -2332,7 +2360,7 @@
         <v>83</v>
       </c>
       <c r="G102" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.35">
@@ -2346,7 +2374,7 @@
         <v>83</v>
       </c>
       <c r="G103" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.35">
@@ -2360,7 +2388,7 @@
         <v>83</v>
       </c>
       <c r="G104" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.35">
@@ -2475,12 +2503,12 @@
         <v>139</v>
       </c>
       <c r="G116" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E117" t="s">
         <v>140</v>
@@ -2622,7 +2650,7 @@
         <v>83</v>
       </c>
       <c r="G129" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.35">
@@ -3113,9 +3141,6 @@
       <c r="E178" t="s">
         <v>4</v>
       </c>
-      <c r="F178" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C179" t="s">
@@ -3124,9 +3149,6 @@
       <c r="E179" t="s">
         <v>224</v>
       </c>
-      <c r="F179" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C180" t="s">
@@ -3135,12 +3157,6 @@
       <c r="E180" t="s">
         <v>225</v>
       </c>
-      <c r="F180" t="s">
-        <v>223</v>
-      </c>
-      <c r="G180" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C181" t="s">
@@ -3149,9 +3165,6 @@
       <c r="E181" t="s">
         <v>226</v>
       </c>
-      <c r="F181" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C182" t="s">
@@ -3160,12 +3173,6 @@
       <c r="E182" t="s">
         <v>227</v>
       </c>
-      <c r="F182" t="s">
-        <v>83</v>
-      </c>
-      <c r="G182" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="183" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C183" t="s">
@@ -3174,9 +3181,6 @@
       <c r="E183" t="s">
         <v>228</v>
       </c>
-      <c r="F183" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="184" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
@@ -3198,7 +3202,21 @@
         <v>207</v>
       </c>
     </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B192" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C192" s="7"/>
+      <c r="D192" s="7"/>
+      <c r="E192" s="7"/>
+      <c r="F192" s="7"/>
+      <c r="G192" s="7"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B192:G192"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added tests for mirspectrum for the options Terhardt, ToivianinenSnyder, Fluctuation, Cents, Collapsed, Mel, Bands, Bark and Mask
</commit_message>
<xml_diff>
--- a/migrationTest/migration.xlsb.xlsx
+++ b/migrationTest/migration.xlsb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emon1\Documents\MATLAB\toolbox\miningsuite\migrationTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hr193\Documents\MATLAB\toolbox\miningsuite\migrationTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57544F70-04D9-46A0-A026-4CEED90D2FFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4EB445-544D-4515-894F-59AB28CEE8DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="19200" windowHeight="8510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2240" yWindow="2150" windowWidth="16330" windowHeight="9390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="228">
   <si>
     <t>mirtoolbox</t>
   </si>
@@ -660,42 +660,9 @@
     <t>aud.envelope</t>
   </si>
   <si>
-    <t>maximum absolute difference : 0.0033392</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 0.00014749</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 5.4251e-06</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 3.8529e-07</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 5.632e-11</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 5.6844e-11</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 1.0378e-05</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 8529e-07</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 2.5121e-05</t>
-  </si>
-  <si>
-    <t>maximum absolute difference : 1.7906e-12</t>
-  </si>
-  <si>
     <t>maximum absolute difference : 12327.9033</t>
   </si>
   <si>
-    <t>maximum absolute difference : 4.0075e-12</t>
-  </si>
-  <si>
     <t>SUCCESS</t>
   </si>
   <si>
@@ -714,30 +681,6 @@
     <t>…, 'RMS'</t>
   </si>
   <si>
-    <t>maximum absolute difference: 0.00037173</t>
-  </si>
-  <si>
-    <t>value in miningsuite = 10 x value in mirtoolbox</t>
-  </si>
-  <si>
-    <t>significant data error</t>
-  </si>
-  <si>
-    <t>dimension error (596, 595)</t>
-  </si>
-  <si>
-    <t>significant dimension error (131073, 130800); values significantly different</t>
-  </si>
-  <si>
-    <t>dimension error(131073, 131074)</t>
-  </si>
-  <si>
-    <t>dimension error(11517, 11518)</t>
-  </si>
-  <si>
-    <t>significant dimension error (11517, 11532)</t>
-  </si>
-  <si>
     <t>implementation error</t>
   </si>
   <si>
@@ -751,6 +694,21 @@
   </si>
   <si>
     <t>Feature Extractors</t>
+  </si>
+  <si>
+    <t>dimension error (mirtoolbox is 1 cell short). Mirtoolbox is faulty here</t>
+  </si>
+  <si>
+    <t>insignificant differences</t>
+  </si>
+  <si>
+    <t>aud.spectrum</t>
+  </si>
+  <si>
+    <t>mus.spectrum</t>
+  </si>
+  <si>
+    <t>significant data differences</t>
   </si>
 </sst>
 </file>
@@ -1170,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B130" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView tabSelected="1" topLeftCell="B91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1212,7 +1170,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1240,7 +1198,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
@@ -1251,7 +1209,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
@@ -1262,7 +1220,7 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
@@ -1273,7 +1231,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
@@ -1292,7 +1250,7 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
@@ -1303,7 +1261,7 @@
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
@@ -1314,7 +1272,7 @@
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.35">
@@ -1325,7 +1283,7 @@
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.35">
@@ -1344,7 +1302,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
@@ -1355,7 +1313,7 @@
         <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
@@ -1366,7 +1324,7 @@
         <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
@@ -1377,7 +1335,7 @@
         <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
@@ -1388,7 +1346,7 @@
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
@@ -1423,7 +1381,7 @@
         <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
@@ -1434,7 +1392,7 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
@@ -1445,7 +1403,7 @@
         <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.35">
@@ -1456,7 +1414,7 @@
         <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
@@ -1467,7 +1425,7 @@
         <v>40</v>
       </c>
       <c r="F26" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
@@ -1478,7 +1436,7 @@
         <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
@@ -1489,7 +1447,7 @@
         <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
@@ -1512,7 +1470,7 @@
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
@@ -1526,7 +1484,7 @@
         <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
@@ -1540,7 +1498,7 @@
         <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
@@ -1554,7 +1512,7 @@
         <v>51</v>
       </c>
       <c r="F33" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.35">
@@ -1568,7 +1526,7 @@
         <v>52</v>
       </c>
       <c r="F34" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.35">
@@ -1582,7 +1540,7 @@
         <v>27</v>
       </c>
       <c r="F35" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.35">
@@ -1596,7 +1554,7 @@
         <v>55</v>
       </c>
       <c r="F36" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
@@ -1610,7 +1568,7 @@
         <v>57</v>
       </c>
       <c r="F37" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.35">
@@ -1624,7 +1582,7 @@
         <v>59</v>
       </c>
       <c r="F38" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
@@ -1638,7 +1596,7 @@
         <v>61</v>
       </c>
       <c r="F39" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.35">
@@ -1652,7 +1610,7 @@
         <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.35">
@@ -1666,7 +1624,7 @@
         <v>64</v>
       </c>
       <c r="F41" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.35">
@@ -1680,7 +1638,7 @@
         <v>65</v>
       </c>
       <c r="F42" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.35">
@@ -1694,7 +1652,7 @@
         <v>66</v>
       </c>
       <c r="F43" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.35">
@@ -1708,7 +1666,7 @@
         <v>67</v>
       </c>
       <c r="F44" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.35">
@@ -1731,7 +1689,7 @@
         <v>70</v>
       </c>
       <c r="F46" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
@@ -1742,7 +1700,7 @@
         <v>71</v>
       </c>
       <c r="F47" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.35">
@@ -1753,7 +1711,7 @@
         <v>72</v>
       </c>
       <c r="F48" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.35">
@@ -1764,7 +1722,7 @@
         <v>73</v>
       </c>
       <c r="F49" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.35">
@@ -1775,7 +1733,7 @@
         <v>74</v>
       </c>
       <c r="F50" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.35">
@@ -1786,7 +1744,7 @@
         <v>75</v>
       </c>
       <c r="F51" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.35">
@@ -1797,7 +1755,7 @@
         <v>76</v>
       </c>
       <c r="F52" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.35">
@@ -1808,7 +1766,7 @@
         <v>77</v>
       </c>
       <c r="F53" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.35">
@@ -1819,7 +1777,7 @@
         <v>78</v>
       </c>
       <c r="F54" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.35">
@@ -1830,7 +1788,7 @@
         <v>79</v>
       </c>
       <c r="F55" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.35">
@@ -1876,7 +1834,7 @@
         <v>209</v>
       </c>
       <c r="F60" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.35">
@@ -1887,7 +1845,7 @@
         <v>84</v>
       </c>
       <c r="F61" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.35">
@@ -1898,7 +1856,7 @@
         <v>85</v>
       </c>
       <c r="F62" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.35">
@@ -1909,7 +1867,7 @@
         <v>86</v>
       </c>
       <c r="F63" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.35">
@@ -1929,7 +1887,7 @@
         <v>88</v>
       </c>
       <c r="F65" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.35">
@@ -1940,7 +1898,7 @@
         <v>89</v>
       </c>
       <c r="F66" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.35">
@@ -1951,7 +1909,7 @@
         <v>90</v>
       </c>
       <c r="F67" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.35">
@@ -1962,7 +1920,7 @@
         <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.35">
@@ -1973,7 +1931,7 @@
         <v>91</v>
       </c>
       <c r="F69" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.35">
@@ -1984,7 +1942,7 @@
         <v>92</v>
       </c>
       <c r="F70" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.35">
@@ -1995,7 +1953,7 @@
         <v>93</v>
       </c>
       <c r="F71" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.35">
@@ -2009,7 +1967,7 @@
         <v>94</v>
       </c>
       <c r="F72" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.35">
@@ -2020,7 +1978,7 @@
         <v>95</v>
       </c>
       <c r="F73" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.35">
@@ -2034,7 +1992,7 @@
         <v>83</v>
       </c>
       <c r="G74" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.35">
@@ -2048,7 +2006,7 @@
         <v>83</v>
       </c>
       <c r="G75" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.35">
@@ -2059,7 +2017,7 @@
         <v>11</v>
       </c>
       <c r="F76" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.35">
@@ -2073,7 +2031,7 @@
         <v>83</v>
       </c>
       <c r="G77" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.35">
@@ -2087,7 +2045,7 @@
         <v>99</v>
       </c>
       <c r="F78" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.35">
@@ -2098,10 +2056,7 @@
         <v>100</v>
       </c>
       <c r="F79" t="s">
-        <v>83</v>
-      </c>
-      <c r="G79" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.35">
@@ -2112,18 +2067,21 @@
         <v>101</v>
       </c>
       <c r="F80" t="s">
-        <v>83</v>
-      </c>
-      <c r="G80" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C81" t="s">
         <v>102</v>
       </c>
+      <c r="E81" t="s">
+        <v>102</v>
+      </c>
       <c r="F81" t="s">
-        <v>12</v>
+        <v>82</v>
+      </c>
+      <c r="G81" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.35">
@@ -2136,7 +2094,7 @@
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="G82" s="5"/>
     </row>
@@ -2148,7 +2106,7 @@
         <v>105</v>
       </c>
       <c r="F83" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.35">
@@ -2159,7 +2117,7 @@
         <v>106</v>
       </c>
       <c r="F84" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.35">
@@ -2170,10 +2128,10 @@
         <v>107</v>
       </c>
       <c r="F85" t="s">
-        <v>83</v>
+        <v>212</v>
       </c>
       <c r="G85" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.35">
@@ -2184,7 +2142,7 @@
         <v>108</v>
       </c>
       <c r="F86" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.35">
@@ -2195,7 +2153,7 @@
         <v>109</v>
       </c>
       <c r="F87" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.35">
@@ -2206,7 +2164,7 @@
         <v>110</v>
       </c>
       <c r="F88" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.35">
@@ -2217,10 +2175,7 @@
         <v>111</v>
       </c>
       <c r="F89" t="s">
-        <v>83</v>
-      </c>
-      <c r="G89" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.35">
@@ -2231,7 +2186,7 @@
         <v>112</v>
       </c>
       <c r="F90" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.35">
@@ -2242,7 +2197,7 @@
         <v>113</v>
       </c>
       <c r="F91" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.35">
@@ -2253,7 +2208,7 @@
         <v>114</v>
       </c>
       <c r="F92" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.35">
@@ -2264,7 +2219,7 @@
         <v>115</v>
       </c>
       <c r="F93" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.35">
@@ -2275,15 +2230,24 @@
         <v>116</v>
       </c>
       <c r="F94" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C95" t="s">
         <v>117</v>
       </c>
+      <c r="D95" t="s">
+        <v>225</v>
+      </c>
+      <c r="E95" t="s">
+        <v>117</v>
+      </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>212</v>
+      </c>
+      <c r="G95" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.35">
@@ -2294,7 +2258,7 @@
         <v>118</v>
       </c>
       <c r="F96" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.35">
@@ -2305,10 +2269,10 @@
         <v>119</v>
       </c>
       <c r="F97" t="s">
-        <v>83</v>
+        <v>212</v>
       </c>
       <c r="G97" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.35">
@@ -2319,7 +2283,7 @@
         <v>120</v>
       </c>
       <c r="F98" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.35">
@@ -2330,23 +2294,41 @@
         <v>121</v>
       </c>
       <c r="F99" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C100" t="s">
         <v>122</v>
       </c>
+      <c r="D100" t="s">
+        <v>226</v>
+      </c>
+      <c r="E100" t="s">
+        <v>122</v>
+      </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>212</v>
+      </c>
+      <c r="G100" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
         <v>123</v>
       </c>
+      <c r="D101" t="s">
+        <v>226</v>
+      </c>
+      <c r="E101" t="s">
+        <v>123</v>
+      </c>
       <c r="F101" t="s">
-        <v>12</v>
+        <v>212</v>
+      </c>
+      <c r="G101" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.35">
@@ -2357,10 +2339,7 @@
         <v>124</v>
       </c>
       <c r="F102" t="s">
-        <v>83</v>
-      </c>
-      <c r="G102" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.35">
@@ -2371,10 +2350,7 @@
         <v>125</v>
       </c>
       <c r="F103" t="s">
-        <v>83</v>
-      </c>
-      <c r="G103" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.35">
@@ -2385,58 +2361,97 @@
         <v>126</v>
       </c>
       <c r="F104" t="s">
-        <v>83</v>
-      </c>
-      <c r="G104" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>127</v>
       </c>
+      <c r="D105" t="s">
+        <v>226</v>
+      </c>
       <c r="F105" t="s">
-        <v>12</v>
+        <v>83</v>
+      </c>
+      <c r="G105" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>128</v>
       </c>
+      <c r="D106" t="s">
+        <v>226</v>
+      </c>
       <c r="F106" t="s">
-        <v>12</v>
+        <v>83</v>
+      </c>
+      <c r="G106" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
         <v>129</v>
       </c>
+      <c r="D107" t="s">
+        <v>225</v>
+      </c>
+      <c r="E107" t="s">
+        <v>129</v>
+      </c>
       <c r="F107" t="s">
-        <v>12</v>
+        <v>212</v>
+      </c>
+      <c r="G107" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>130</v>
       </c>
+      <c r="D108" t="s">
+        <v>225</v>
+      </c>
+      <c r="E108" t="s">
+        <v>130</v>
+      </c>
       <c r="F108" t="s">
-        <v>12</v>
+        <v>212</v>
       </c>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
         <v>131</v>
       </c>
+      <c r="D109" t="s">
+        <v>225</v>
+      </c>
+      <c r="E109" t="s">
+        <v>131</v>
+      </c>
       <c r="F109" t="s">
-        <v>12</v>
+        <v>212</v>
+      </c>
+      <c r="G109" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
         <v>132</v>
       </c>
+      <c r="D110" t="s">
+        <v>225</v>
+      </c>
+      <c r="E110" t="s">
+        <v>132</v>
+      </c>
       <c r="F110" t="s">
-        <v>12</v>
+        <v>212</v>
       </c>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.35">
@@ -2447,7 +2462,7 @@
         <v>133</v>
       </c>
       <c r="F111" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.35">
@@ -2458,7 +2473,7 @@
         <v>134</v>
       </c>
       <c r="F112" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.35">
@@ -2480,8 +2495,11 @@
       <c r="E114" t="s">
         <v>137</v>
       </c>
+      <c r="F114" t="s">
+        <v>212</v>
+      </c>
       <c r="G114" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.35">
@@ -2491,8 +2509,11 @@
       <c r="E115" t="s">
         <v>138</v>
       </c>
+      <c r="F115" t="s">
+        <v>83</v>
+      </c>
       <c r="G115" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.35">
@@ -2502,19 +2523,25 @@
       <c r="E116" t="s">
         <v>139</v>
       </c>
+      <c r="F116" t="s">
+        <v>83</v>
+      </c>
       <c r="G116" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="E117" t="s">
         <v>140</v>
       </c>
+      <c r="F117" t="s">
+        <v>212</v>
+      </c>
       <c r="G117" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.35">
@@ -2525,7 +2552,7 @@
         <v>141</v>
       </c>
       <c r="F118" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.35">
@@ -2547,8 +2574,11 @@
       <c r="E120" t="s">
         <v>105</v>
       </c>
+      <c r="F120" t="s">
+        <v>212</v>
+      </c>
       <c r="G120" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
     </row>
     <row r="121" spans="2:7" x14ac:dyDescent="0.35">
@@ -2558,8 +2588,11 @@
       <c r="E121" t="s">
         <v>106</v>
       </c>
+      <c r="F121" t="s">
+        <v>212</v>
+      </c>
       <c r="G121" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="2:7" x14ac:dyDescent="0.35">
@@ -2569,8 +2602,11 @@
       <c r="E122" t="s">
         <v>144</v>
       </c>
+      <c r="F122" t="s">
+        <v>212</v>
+      </c>
       <c r="G122" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.35">
@@ -2580,8 +2616,11 @@
       <c r="E123" t="s">
         <v>145</v>
       </c>
+      <c r="F123" t="s">
+        <v>212</v>
+      </c>
       <c r="G123" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.35">
@@ -2591,8 +2630,11 @@
       <c r="E124" t="s">
         <v>146</v>
       </c>
+      <c r="F124" t="s">
+        <v>212</v>
+      </c>
       <c r="G124" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.35">
@@ -2602,8 +2644,11 @@
       <c r="E125" t="s">
         <v>147</v>
       </c>
+      <c r="F125" t="s">
+        <v>212</v>
+      </c>
       <c r="G125" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
     </row>
     <row r="126" spans="2:7" x14ac:dyDescent="0.35">
@@ -2613,8 +2658,11 @@
       <c r="E126" t="s">
         <v>148</v>
       </c>
+      <c r="F126" t="s">
+        <v>212</v>
+      </c>
       <c r="G126" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.35">
@@ -2624,8 +2672,11 @@
       <c r="E127" t="s">
         <v>149</v>
       </c>
+      <c r="F127" t="s">
+        <v>212</v>
+      </c>
       <c r="G127" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.35">
@@ -2635,8 +2686,11 @@
       <c r="E128" t="s">
         <v>150</v>
       </c>
+      <c r="F128" t="s">
+        <v>212</v>
+      </c>
       <c r="G128" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.35">
@@ -2650,7 +2704,7 @@
         <v>83</v>
       </c>
       <c r="G129" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.35">
@@ -2673,8 +2727,11 @@
       <c r="E132" t="s">
         <v>153</v>
       </c>
+      <c r="F132" t="s">
+        <v>212</v>
+      </c>
       <c r="G132" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.35">
@@ -2685,7 +2742,7 @@
         <v>154</v>
       </c>
       <c r="F133" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.35">
@@ -2705,8 +2762,11 @@
       <c r="E136" t="s">
         <v>157</v>
       </c>
+      <c r="F136" t="s">
+        <v>212</v>
+      </c>
       <c r="G136" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.35">
@@ -2716,8 +2776,11 @@
       <c r="E137" t="s">
         <v>158</v>
       </c>
+      <c r="F137" t="s">
+        <v>212</v>
+      </c>
       <c r="G137" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.35">
@@ -2751,7 +2814,7 @@
         <v>137</v>
       </c>
       <c r="F140" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.35">
@@ -2762,7 +2825,7 @@
         <v>162</v>
       </c>
       <c r="F141" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.35">
@@ -2773,7 +2836,7 @@
         <v>163</v>
       </c>
       <c r="F142" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.35">
@@ -2784,7 +2847,7 @@
         <v>141</v>
       </c>
       <c r="F143" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.35">
@@ -2839,7 +2902,7 @@
         <v>170</v>
       </c>
       <c r="F149" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.35">
@@ -2850,7 +2913,7 @@
         <v>172</v>
       </c>
       <c r="F150" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.35">
@@ -2884,7 +2947,7 @@
         <v>4</v>
       </c>
       <c r="F153" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.35">
@@ -2895,7 +2958,7 @@
         <v>177</v>
       </c>
       <c r="F154" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.35">
@@ -2906,7 +2969,7 @@
         <v>178</v>
       </c>
       <c r="F155" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="156" spans="2:7" x14ac:dyDescent="0.35">
@@ -2917,7 +2980,7 @@
         <v>179</v>
       </c>
       <c r="F156" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.35">
@@ -2928,7 +2991,7 @@
         <v>180</v>
       </c>
       <c r="F157" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.35">
@@ -2939,7 +3002,7 @@
         <v>181</v>
       </c>
       <c r="F158" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.35">
@@ -2950,7 +3013,7 @@
         <v>182</v>
       </c>
       <c r="F159" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="160" spans="2:7" x14ac:dyDescent="0.35">
@@ -2961,7 +3024,7 @@
         <v>183</v>
       </c>
       <c r="F160" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="161" spans="3:6" x14ac:dyDescent="0.35">
@@ -2972,7 +3035,7 @@
         <v>184</v>
       </c>
       <c r="F161" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="162" spans="3:6" x14ac:dyDescent="0.35">
@@ -2983,7 +3046,7 @@
         <v>185</v>
       </c>
       <c r="F162" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="163" spans="3:6" x14ac:dyDescent="0.35">
@@ -2994,7 +3057,7 @@
         <v>186</v>
       </c>
       <c r="F163" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="164" spans="3:6" x14ac:dyDescent="0.35">
@@ -3005,7 +3068,7 @@
         <v>187</v>
       </c>
       <c r="F164" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="165" spans="3:6" x14ac:dyDescent="0.35">
@@ -3016,7 +3079,7 @@
         <v>188</v>
       </c>
       <c r="F165" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="166" spans="3:6" x14ac:dyDescent="0.35">
@@ -3027,7 +3090,7 @@
         <v>189</v>
       </c>
       <c r="F166" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="167" spans="3:6" x14ac:dyDescent="0.35">
@@ -3038,7 +3101,7 @@
         <v>190</v>
       </c>
       <c r="F167" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="168" spans="3:6" x14ac:dyDescent="0.35">
@@ -3049,7 +3112,7 @@
         <v>191</v>
       </c>
       <c r="F168" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="169" spans="3:6" x14ac:dyDescent="0.35">
@@ -3078,7 +3141,7 @@
         <v>194</v>
       </c>
       <c r="F171" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="172" spans="3:6" x14ac:dyDescent="0.35">
@@ -3089,7 +3152,7 @@
         <v>195</v>
       </c>
       <c r="F172" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="173" spans="3:6" x14ac:dyDescent="0.35">
@@ -3144,42 +3207,42 @@
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C179" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="E179" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C180" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="E180" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C181" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E181" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C182" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="E182" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="183" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C183" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="E183" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="184" spans="2:7" x14ac:dyDescent="0.35">
@@ -3204,7 +3267,7 @@
     </row>
     <row r="192" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B192" s="7" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="C192" s="7"/>
       <c r="D192" s="7"/>

</xml_diff>